<commit_message>
Update school year dates in YearEndReconciliation template to 2021-2022.
</commit_message>
<xml_diff>
--- a/SchoolDistrictBilling/wwwroot/reportTemplates/YearEndReconciliation.xlsx
+++ b/SchoolDistrictBilling/wwwroot/reportTemplates/YearEndReconciliation.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Out of District Billing\FY19.20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhensinger/dev/omnivest/SdBilling/SchoolDistrictBilling/wwwroot/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDB58561-3C85-44B3-B314-AD5D8CE8C82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Prior Year Reconciliation" sheetId="3" r:id="rId1"/>
@@ -18,8 +17,14 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Prior Year Reconciliation'!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -112,24 +117,6 @@
   </si>
   <si>
     <t>Reconciliation Prep Date:</t>
-  </si>
-  <si>
-    <t>RECONCILIATION REPORT FOR THE 2019-2020 SCHOOL YEAR</t>
-  </si>
-  <si>
-    <t>Total Amount Due for 2019-2020 School Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          Total Amount Due for 2019-2020 School Year:</t>
-  </si>
-  <si>
-    <t>July, 2019</t>
-  </si>
-  <si>
-    <t>January, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Total Paid to Date for 2019-2020 School Year:</t>
   </si>
   <si>
     <t>Selected
@@ -158,7 +145,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Days Membership</t>
@@ -167,10 +153,6 @@
   <si>
     <t>Charter School
 Days in Session</t>
-  </si>
-  <si>
-    <t>1.  Do not include students that enrolled after
-     March 13, 2020.</t>
   </si>
   <si>
     <r>
@@ -200,11 +182,33 @@
       <t xml:space="preserve"> 1</t>
     </r>
   </si>
+  <si>
+    <t>RECONCILIATION REPORT FOR THE 2021-2022 SCHOOL YEAR</t>
+  </si>
+  <si>
+    <t>Total Amount Due for 2021-2022 School Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Total Amount Due for 2021-2022 School Year:</t>
+  </si>
+  <si>
+    <t>July, 2021</t>
+  </si>
+  <si>
+    <t>January, 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Total Paid to Date for 2021-2022 School Year:</t>
+  </si>
+  <si>
+    <t>1.  Do not include students that enrolled after
+     March 13, 2022.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -304,7 +308,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -312,7 +316,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -418,7 +422,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -433,7 +437,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -446,7 +450,7 @@
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -488,7 +492,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,7 +507,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,7 +520,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -694,6 +698,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,9 +844,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -867,31 +874,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -919,23 +909,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1111,24 +1084,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA528FB4-7180-40F7-819E-DDC280515654}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="18.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="5" max="7" width="18.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1140,19 +1115,19 @@
       <c r="H1" s="20"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="E2" s="14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -1164,7 +1139,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1175,7 +1150,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="55" t="s">
         <v>19</v>
       </c>
@@ -1191,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="55" t="s">
         <v>20</v>
       </c>
@@ -1207,7 +1182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="16"/>
@@ -1221,29 +1196,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="43.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C9" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="28" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="54" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B10" s="54"/>
       <c r="C10" s="50"/>
@@ -1259,9 +1234,9 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:10" s="28" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="54" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B11" s="54"/>
       <c r="C11" s="50"/>
@@ -1277,20 +1252,20 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G12" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H12" s="9">
         <f>ROUND(SUM(H10:H11),2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C15" s="11" t="s">
         <v>1</v>
       </c>
@@ -1308,9 +1283,9 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C16" s="22" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="42"/>
@@ -1318,7 +1293,7 @@
       <c r="G16" s="43"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C17" s="23" t="s">
         <v>6</v>
       </c>
@@ -1327,7 +1302,7 @@
       <c r="F17" s="45"/>
       <c r="G17" s="46"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C18" s="24" t="s">
         <v>7</v>
       </c>
@@ -1336,7 +1311,7 @@
       <c r="F18" s="45"/>
       <c r="G18" s="46"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C19" s="24" t="s">
         <v>8</v>
       </c>
@@ -1345,7 +1320,7 @@
       <c r="F19" s="45"/>
       <c r="G19" s="46"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C20" s="24" t="s">
         <v>9</v>
       </c>
@@ -1354,7 +1329,7 @@
       <c r="F20" s="45"/>
       <c r="G20" s="46"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C21" s="24" t="s">
         <v>10</v>
       </c>
@@ -1363,16 +1338,16 @@
       <c r="F21" s="45"/>
       <c r="G21" s="46"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C22" s="24" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
       <c r="G22" s="46"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C23" s="30" t="s">
         <v>11</v>
       </c>
@@ -1381,7 +1356,7 @@
       <c r="F23" s="45"/>
       <c r="G23" s="46"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C24" s="24" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1365,7 @@
       <c r="F24" s="45"/>
       <c r="G24" s="46"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C25" s="24" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1374,7 @@
       <c r="F25" s="45"/>
       <c r="G25" s="46"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C26" s="24" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1383,7 @@
       <c r="F26" s="45"/>
       <c r="G26" s="46"/>
     </row>
-    <row r="27" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C27" s="25" t="s">
         <v>5</v>
       </c>
@@ -1417,7 +1392,7 @@
       <c r="F27" s="48"/>
       <c r="G27" s="49"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D28" s="6"/>
       <c r="E28" s="6">
         <f>SUM(E16:E27)</f>
@@ -1432,26 +1407,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G30" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H30" s="9">
         <f>E28+F28-G28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="53"/>
       <c r="B32" s="54"/>
       <c r="C32" s="54"/>
@@ -1464,19 +1439,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="54"/>
       <c r="B33" s="54"/>
       <c r="C33" s="54"/>
     </row>
-    <row r="34" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="53" t="s">
-        <v>36</v>
+    <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="56" t="s">
+        <v>38</v>
       </c>
       <c r="B34" s="54"/>
       <c r="C34" s="54"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="54"/>
       <c r="B35" s="54"/>
       <c r="C35" s="54"/>
@@ -1508,23 +1483,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Category xmlns="b422c1b9-d571-47a6-807c-ec0c6274877e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063A4E9D8B9AE294BB8664582FC3229C4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3494bfc67ca4592f34fccaac583e2a82">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b422c1b9-d571-47a6-807c-ec0c6274877e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd6863714e329a50f96a79b1cd1d8a06" ns2:_="">
     <xsd:import namespace="b422c1b9-d571-47a6-807c-ec0c6274877e"/>
@@ -1652,7 +1610,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Category xmlns="b422c1b9-d571-47a6-807c-ec0c6274877e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E72C0A9-3335-4C82-87B0-FA04DDB774A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b422c1b9-d571-47a6-807c-ec0c6274877e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406E8E76-4311-4627-98FC-776FC991A1F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1660,7 +1653,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2659C8-FE49-43FD-B7C1-93B083A2EF67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1676,22 +1669,4 @@
     <ds:schemaRef ds:uri="b422c1b9-d571-47a6-807c-ec0c6274877e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E72C0A9-3335-4C82-87B0-FA04DDB774A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b422c1b9-d571-47a6-807c-ec0c6274877e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to year end reconciliation form for 22-23 school year.
</commit_message>
<xml_diff>
--- a/SchoolDistrictBilling/wwwroot/reportTemplates/YearEndReconciliation.xlsx
+++ b/SchoolDistrictBilling/wwwroot/reportTemplates/YearEndReconciliation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200"/>
   </bookViews>
   <sheets>
     <sheet name="Prior Year Reconciliation" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Average Daily Membership</t>
   </si>
@@ -183,26 +183,22 @@
     </r>
   </si>
   <si>
-    <t>RECONCILIATION REPORT FOR THE 2021-2022 SCHOOL YEAR</t>
-  </si>
-  <si>
-    <t>Total Amount Due for 2021-2022 School Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          Total Amount Due for 2021-2022 School Year:</t>
-  </si>
-  <si>
-    <t>July, 2021</t>
-  </si>
-  <si>
-    <t>January, 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Total Paid to Date for 2021-2022 School Year:</t>
-  </si>
-  <si>
-    <t>1.  Do not include students that enrolled after
-     March 13, 2022.</t>
+    <t>RECONCILIATION REPORT FOR THE 2022-2023 SCHOOL YEAR</t>
+  </si>
+  <si>
+    <t>Total Amount Due for 2022-2023 School Year</t>
+  </si>
+  <si>
+    <t>July, 2022</t>
+  </si>
+  <si>
+    <t>January, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Total Paid to Date for 2022-2023 School Year:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Total Amount Due for 2022-2023 School Year:</t>
   </si>
 </sst>
 </file>
@@ -214,7 +210,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -280,6 +276,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -528,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -689,18 +694,37 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1088,15 +1112,15 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
     <col min="5" max="7" width="18.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
@@ -1111,8 +1135,8 @@
         <v>12</v>
       </c>
       <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="58"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
@@ -1123,8 +1147,8 @@
         <v>32</v>
       </c>
       <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -1135,8 +1159,8 @@
         <v>15</v>
       </c>
       <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -1146,15 +1170,15 @@
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="55"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="12"/>
@@ -1167,10 +1191,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="12"/>
@@ -1254,7 +1278,7 @@
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G12" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H12" s="9">
         <f>ROUND(SUM(H10:H11),2)</f>
@@ -1285,7 +1309,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C16" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="42"/>
@@ -1340,7 +1364,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C22" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="45"/>
@@ -1414,7 +1438,7 @@
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G30" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H30" s="9">
         <f>E28+F28-G28</f>
@@ -1427,7 +1451,7 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="53"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="54"/>
       <c r="C32" s="54"/>
       <c r="G32" s="26" t="str">
@@ -1445,9 +1469,7 @@
       <c r="C33" s="54"/>
     </row>
     <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="56" t="s">
-        <v>38</v>
-      </c>
+      <c r="A34" s="53"/>
       <c r="B34" s="54"/>
       <c r="C34" s="54"/>
     </row>

</xml_diff>